<commit_message>
criação dee arquivo csv implemenada
</commit_message>
<xml_diff>
--- a/planilha-lorem.xlsx
+++ b/planilha-lorem.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>tipo de alimento</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>bacon</t>
+  </si>
+  <si>
+    <t>vaca</t>
   </si>
 </sst>
 </file>
@@ -288,6 +291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -334,7 +338,15 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>